<commit_message>
✨ Adding complete test plans
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EDA083-F19D-4139-8621-4DA260D5624C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1DCE07-FB3E-44A7-9197-6C2417FEB91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanDePruebaPapaJohn's" sheetId="2" r:id="rId1"/>
@@ -156,19 +156,6 @@
     <t>Informar del defecto al equipo de desarrollo.</t>
   </si>
   <si>
-    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 27 de febrero en las horas 12:00 PM a 01:00 PM.</t>
-  </si>
-  <si>
-    <t>Se supone que solo se permite el registro de usuarios que están en la lista de la página.</t>
-  </si>
-  <si>
-    <t>Funcionamiento de los microservicios de la pagina reqres.in.</t>
-  </si>
-  <si>
-    <t>Se recomienda ejecutar pruebas de seguridad.
-Se recomienda ejecutar pruebas de rendimiento.</t>
-  </si>
-  <si>
     <t>Metodo Gherkin:</t>
   </si>
   <si>
@@ -2083,9 +2070,6 @@
 </t>
   </si>
   <si>
-    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 4 de Marzo en las horas de 09:00 AM a 05:00 PM.</t>
-  </si>
-  <si>
     <t>Tener una cuenta válida en la página de domicilios de Papa John´s.</t>
   </si>
   <si>
@@ -2150,9 +2134,26 @@
     </r>
   </si>
   <si>
-    <t>Se probará la respuesta de la petición.
-Se probará el URL de la petición realizando cambios en los campos de correo "name.last@reqres.in" y contraseña "pass123".
-Se realizarán peticiones con diferentes estructuras en el cuerpo a enviar.
+    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 4 de marzo en las horas de 09:00 AM a 05:00 PM.</t>
+  </si>
+  <si>
+    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 5 de marzo en las horas de 08:00 AM a 05:00 PM.</t>
+  </si>
+  <si>
+    <t>Tener una cuenta en Xignite con acceso a los servicios SOAP de conversión de moneda y tasa de cambio.</t>
+  </si>
+  <si>
+    <t>Se recomienda ejecutar pruebas de seguridad, debido a la presencia de un token de autenticación generado en la página de Xignite.
+Se recomienda ejecutar pruebas de estrés, ya que el servicio puede ser utilizado por muchas personas a la vez.</t>
+  </si>
+  <si>
+    <t>Se supone que Xignite permite realizar peticiones desde el cliente SOAP UI.</t>
+  </si>
+  <si>
+    <t>Se probarán las respuestas de las peticiones sin un token de autenticación válido.
+Se probarán las peticiones realizando cambios válidos y no válidos en los campos no obligatorios de Username, Password, Tracer, From, To, Country, Symbol y AsOfDate.
+Se probará la petición de conversión de moneda, realizando cambios válidos y no válidos en el campo Amount.
+Se realizará una comprobación de las respuestas recibidas por los servicios.
 Todas las pruebas serán ejecutadas manualmente, y como no se conoce el funcionamiento interno de los servicios de conversión de moneda y tasa de cambio, todas las estrategias de prueba serán de caja negra.</t>
   </si>
 </sst>
@@ -2899,7 +2900,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3015,12 +3016,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3147,7 +3148,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3499,15 +3499,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>519622</xdr:colOff>
+      <xdr:colOff>463018</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>56604</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>22154</xdr:rowOff>
+      <xdr:rowOff>8964</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3522,7 +3522,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -3530,14 +3530,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect t="24358" b="21755"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11337301" y="231321"/>
-          <a:ext cx="2868555" cy="1219583"/>
+          <a:off x="12574336" y="233082"/>
+          <a:ext cx="2853923" cy="654423"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3983,8 +3982,9 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3997,55 +3997,55 @@
     <col min="6" max="6" width="52.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="63.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54.44140625" customWidth="1"/>
     <col min="10" max="10" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="33.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-    </row>
-    <row r="2" spans="1:13" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+    </row>
+    <row r="2" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>0</v>
@@ -4077,84 +4077,84 @@
     </row>
     <row r="4" spans="1:13" ht="378" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E4" s="33" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="L4" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="G4" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="H4" s="33" t="s">
+      <c r="M4" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="I4" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="K4" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="L4" s="33" t="s">
-        <v>232</v>
-      </c>
-      <c r="M4" s="33" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="288" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:13" ht="369.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>225</v>
-      </c>
       <c r="C5" s="32" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E5" s="32" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I5" s="32" t="s">
         <v>238</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="K5" s="32" t="s">
-        <v>39</v>
+        <v>235</v>
       </c>
       <c r="L5" s="32" t="s">
-        <v>40</v>
+        <v>236</v>
       </c>
       <c r="M5" s="32" t="s">
-        <v>38</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -4196,7 +4196,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -4245,7 +4245,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>21</v>
@@ -4271,7 +4271,7 @@
         <v>23</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.3">
@@ -4279,10 +4279,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D4" s="33">
         <v>1</v>
@@ -4305,7 +4305,7 @@
         <v>22</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -4830,7 +4830,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -4879,7 +4879,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>21</v>
@@ -4905,7 +4905,7 @@
         <v>23</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.3">
@@ -4913,7 +4913,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>21</v>
@@ -4939,7 +4939,7 @@
         <v>23</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -4981,7 +4981,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C6" s="33" t="s">
         <v>21</v>
@@ -5007,7 +5007,7 @@
         <v>25</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -5015,10 +5015,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D7" s="32">
         <v>1</v>
@@ -5041,7 +5041,7 @@
         <v>35</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -5049,7 +5049,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>21</v>
@@ -5075,7 +5075,7 @@
         <v>23</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -5083,10 +5083,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D9" s="32">
         <v>1</v>
@@ -5109,7 +5109,7 @@
         <v>22</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -5117,7 +5117,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>21</v>
@@ -5143,7 +5143,7 @@
         <v>25</v>
       </c>
       <c r="J10" s="33" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -5151,7 +5151,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C11" s="33" t="s">
         <v>21</v>
@@ -5177,18 +5177,18 @@
         <v>23</v>
       </c>
       <c r="J11" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A12" s="32">
         <v>10</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D12" s="32">
         <v>1</v>
@@ -5211,7 +5211,7 @@
         <v>22</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -5219,7 +5219,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C13" s="33" t="s">
         <v>21</v>
@@ -5245,7 +5245,7 @@
         <v>25</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -5253,7 +5253,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>21</v>
@@ -5279,18 +5279,18 @@
         <v>23</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A15" s="32">
         <v>13</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D15" s="32">
         <v>1</v>
@@ -5313,7 +5313,7 @@
         <v>22</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -5321,7 +5321,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C16" s="33" t="s">
         <v>21</v>
@@ -5347,7 +5347,7 @@
         <v>25</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -5355,7 +5355,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>21</v>
@@ -5381,18 +5381,18 @@
         <v>23</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A18" s="32">
         <v>16</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D18" s="32">
         <v>1</v>
@@ -5415,7 +5415,7 @@
         <v>22</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -5441,9 +5441,9 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -5453,138 +5453,137 @@
     <col min="2" max="2" width="75.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B1" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12"/>
       <c r="B6" s="16"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="19"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="B10" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B11" s="15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
-        <v>57</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="49"/>
       <c r="B13" s="50"/>
-      <c r="D13" s="89"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B14" s="19"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>12</v>
@@ -5596,45 +5595,45 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B21" s="19"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>12</v>
@@ -5646,45 +5645,45 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B28" s="19"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>12</v>
@@ -5696,45 +5695,45 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B35" s="19"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>13</v>
@@ -5770,38 +5769,38 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5810,45 +5809,45 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B7" s="19"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>12</v>
@@ -5860,45 +5859,45 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B14" s="19"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>13</v>
@@ -5910,45 +5909,45 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B21" s="19"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>12</v>
@@ -5960,45 +5959,45 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B28" s="19"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>12</v>
@@ -6010,45 +6009,45 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B35" s="19"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>13</v>
@@ -6060,45 +6059,45 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B42" s="19"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>12</v>
@@ -6106,30 +6105,30 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6138,45 +6137,45 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B53" s="14"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>12</v>
@@ -6188,45 +6187,45 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B60" s="19"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B65" s="17" t="s">
         <v>12</v>
@@ -6238,45 +6237,45 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B67" s="19"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B72" s="17" t="s">
         <v>12</v>
@@ -6288,45 +6287,45 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B74" s="19"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>12</v>
@@ -6338,45 +6337,45 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B81" s="19"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B82" s="20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B83" s="20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B84" s="20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B85" s="20" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>12</v>
@@ -6388,45 +6387,45 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B88" s="19"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B89" s="20" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B90" s="20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B91" s="20" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B92" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B93" s="21" t="s">
         <v>13</v>
@@ -6460,94 +6459,94 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:5" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C2" s="55"/>
       <c r="E2" s="28" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C5" s="57"/>
     </row>
     <row r="6" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B6" s="58"/>
       <c r="C6" s="59"/>
     </row>
     <row r="7" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="61"/>
     </row>
     <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C8" s="63"/>
     </row>
     <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="64" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B9" s="65"/>
       <c r="C9" s="66"/>
     </row>
     <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="67" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B10" s="68"/>
       <c r="C10" s="69"/>
     </row>
     <row r="11" spans="1:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="51" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="53"/>
@@ -6560,84 +6559,84 @@
     </row>
     <row r="13" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C13" s="55"/>
     </row>
     <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B16" s="56" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C16" s="57"/>
     </row>
     <row r="17" spans="1:3" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B17" s="58"/>
       <c r="C17" s="59"/>
     </row>
     <row r="18" spans="1:3" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B18" s="60"/>
       <c r="C18" s="61"/>
     </row>
     <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C19" s="63"/>
     </row>
     <row r="20" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="64" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B20" s="65"/>
       <c r="C20" s="66"/>
     </row>
     <row r="21" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B21" s="68"/>
       <c r="C21" s="69"/>
     </row>
     <row r="22" spans="1:3" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="51" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B22" s="52"/>
       <c r="C22" s="53"/>
@@ -6687,94 +6686,94 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
     </row>
     <row r="2" spans="1:5" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C2" s="55"/>
       <c r="E2" s="28" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C5" s="57"/>
     </row>
     <row r="6" spans="1:5" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B6" s="58"/>
       <c r="C6" s="59"/>
     </row>
     <row r="7" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="61"/>
     </row>
     <row r="8" spans="1:5" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C8" s="63"/>
     </row>
     <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="64" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B9" s="65"/>
       <c r="C9" s="66"/>
     </row>
     <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="67" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B10" s="68"/>
       <c r="C10" s="69"/>
     </row>
     <row r="11" spans="1:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="51" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="53"/>
@@ -6786,84 +6785,84 @@
     </row>
     <row r="13" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C13" s="55"/>
     </row>
     <row r="14" spans="1:5" ht="108" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B16" s="56" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C16" s="57"/>
     </row>
     <row r="17" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B17" s="58"/>
       <c r="C17" s="59"/>
     </row>
     <row r="18" spans="1:3" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B18" s="60"/>
       <c r="C18" s="61"/>
     </row>
     <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C19" s="63"/>
     </row>
     <row r="20" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="64" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B20" s="65"/>
       <c r="C20" s="66"/>
     </row>
     <row r="21" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="67" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B21" s="68"/>
       <c r="C21" s="69"/>
     </row>
     <row r="22" spans="1:3" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="51" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B22" s="52"/>
       <c r="C22" s="53"/>
@@ -6875,101 +6874,90 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B24" s="79" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C24" s="80"/>
     </row>
     <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B27" s="81" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C27" s="82"/>
     </row>
     <row r="28" spans="1:3" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B28" s="83"/>
       <c r="C28" s="84"/>
     </row>
     <row r="29" spans="1:3" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B29" s="73"/>
       <c r="C29" s="75"/>
     </row>
     <row r="30" spans="1:3" ht="108" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B30" s="85" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C30" s="72"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="86" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B31" s="87"/>
       <c r="C31" s="88"/>
     </row>
     <row r="32" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="70" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B32" s="71"/>
       <c r="C32" s="72"/>
     </row>
     <row r="33" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="73" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B33" s="74"/>
       <c r="C33" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B5:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B16:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A20:C20"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A23:C23"/>
@@ -6980,6 +6968,17 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B5:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7005,7 +7004,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="42" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -7013,37 +7012,37 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="39" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="38" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="39" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="38" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="39" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="40" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -7051,7 +7050,7 @@
     </row>
     <row r="11" spans="1:1" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="43" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✨ Adding risk matrix for Papa John's
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65973B75-DF4A-495F-80BF-860F2F0590FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8853B655-8A16-4009-A049-40997D020B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="893" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="280">
   <si>
     <t>Plan de Calidad</t>
   </si>
@@ -120,12 +120,6 @@
     <t>Contener</t>
   </si>
   <si>
-    <t>Se registra un usuario con contraseña vacía.</t>
-  </si>
-  <si>
-    <t>Realizar una correcta definición de las reglas para la aceptación de una contraseña como válida.</t>
-  </si>
-  <si>
     <t>Transferir</t>
   </si>
   <si>
@@ -378,40 +372,13 @@
     <t>Método Gherkin:</t>
   </si>
   <si>
-    <t>Fallo del servicio de registro.</t>
-  </si>
-  <si>
-    <t>Fallo del servicio de ingreso.</t>
-  </si>
-  <si>
     <t>Realizar cambio de función del botón en front-end.</t>
   </si>
   <si>
-    <t>El botón de ingreso no funciona.</t>
-  </si>
-  <si>
-    <t>Falta de recursos para el host de la página.</t>
-  </si>
-  <si>
-    <t>Se transfiere la responsabilidad al PO debido a que es un tema económico.</t>
-  </si>
-  <si>
     <t>Los mensajes de error contienen caracteres ilegibles</t>
   </si>
   <si>
     <t>Monitorear la ortografía de los recursos a mostrar en el front-end.</t>
-  </si>
-  <si>
-    <t>Las URL no direccionan donde deberían.</t>
-  </si>
-  <si>
-    <t>Es una característica de la que se encarga el proveedor del host.</t>
-  </si>
-  <si>
-    <t>El botón de crear usuario se bloquea al darle un primer clic.</t>
-  </si>
-  <si>
-    <t>Realizar un control en la función del botón con respecto a la conexión con la BD de usuarios.</t>
   </si>
   <si>
     <t>@MensajeConfirmación</t>
@@ -1944,19 +1911,10 @@
     <t>Responsable Calidad</t>
   </si>
   <si>
-    <t>Analista de Certificación</t>
-  </si>
-  <si>
     <t>Área 1</t>
   </si>
   <si>
     <t>Célula 1</t>
-  </si>
-  <si>
-    <t>Externo</t>
-  </si>
-  <si>
-    <t>Estudiante de SofkaU</t>
   </si>
   <si>
     <t>Célula 2</t>
@@ -2231,6 +2189,96 @@
   </si>
   <si>
     <t>Solicitar la definición WSDL actualizada para el servicio en cuestión.</t>
+  </si>
+  <si>
+    <t>El host de la página se cae</t>
+  </si>
+  <si>
+    <t>Cambiar rápidamente de proveedor de host.</t>
+  </si>
+  <si>
+    <t>La barra de selección de productos está desplazada</t>
+  </si>
+  <si>
+    <t>Hacer que el contenedor de la barra de productos sea adaptable.</t>
+  </si>
+  <si>
+    <t>Se agota el recurso monetario.</t>
+  </si>
+  <si>
+    <t>Informar al PO para evaluar la situación</t>
+  </si>
+  <si>
+    <t>Se porhibe por ley la venta de gaseosas</t>
+  </si>
+  <si>
+    <t>Se elimina la sección de bebidas mientras se realiza un plan de acción desde el área legal de la empresa.</t>
+  </si>
+  <si>
+    <t>Papa John's limita el acceso por no finalizar las compras</t>
+  </si>
+  <si>
+    <t>Se utiliza una cuenta diferente.</t>
+  </si>
+  <si>
+    <t>El usuario no quiere tantos pasos para realizar una compra</t>
+  </si>
+  <si>
+    <t>Informar al PO para que se haga una claridad con respecto a los requerimientos.</t>
+  </si>
+  <si>
+    <t>Jonathan Vargas</t>
+  </si>
+  <si>
+    <t>Falta de experiencia del QA</t>
+  </si>
+  <si>
+    <t>Estudiar más el ISTQB.</t>
+  </si>
+  <si>
+    <t>La estimación de tiempo inicial no se cumple</t>
+  </si>
+  <si>
+    <t>Agilizar la ejecución de pruebas y la escritura de los documentos restantes.</t>
+  </si>
+  <si>
+    <t>Conflictos entre el personal de QA y el PO por falta de actitud de los dos</t>
+  </si>
+  <si>
+    <t>La presentación inicial de ambos equipos, capacitaciones y charlas de motivación y actitud Sofka.</t>
+  </si>
+  <si>
+    <t>El botón de agregar al carro no funciona.</t>
+  </si>
+  <si>
+    <t>Los ingredientes y/o productos en el carro no coinciden con los seleccionados por el cliente</t>
+  </si>
+  <si>
+    <t>Realizar un control en la manera cómo se transfieren los datos de un sistema a otro (del sistema de selección de ingredientes al sistema carro).</t>
+  </si>
+  <si>
+    <t>Las imágenes de los productos se intercambian</t>
+  </si>
+  <si>
+    <t>Informar al personal de desarrollo para que se cambien las fuentes de las imágenes respecto al objeto en el front-end.</t>
+  </si>
+  <si>
+    <t>El botón de editar elimina el producto</t>
+  </si>
+  <si>
+    <t>El cliente puede volver a agregar el mismo producto con los ingredientes deseados.</t>
+  </si>
+  <si>
+    <t>Los productos en el carrito se eliminan al navegar por la página</t>
+  </si>
+  <si>
+    <t>Realizar un control en la persistencia del sistema de carrito.</t>
+  </si>
+  <si>
+    <t>Los productos no favoritos no se pueden agregar al carrito</t>
+  </si>
+  <si>
+    <t>Realizar un control en la funcionalidad de productos favoritos y su relación con el sistema de carrito.</t>
   </si>
 </sst>
 </file>
@@ -3075,7 +3123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3349,6 +3397,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3700,13 +3751,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>463018</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>8964</xdr:rowOff>
@@ -3828,8 +3879,8 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>653143</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4182,11 +4233,11 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:M1"/>
+      <selection pane="bottomLeft" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4194,19 +4245,18 @@
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="63.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="54.44140625" customWidth="1"/>
-    <col min="10" max="10" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.44140625" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="43"/>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -4219,9 +4269,8 @@
       <c r="J1" s="43"/>
       <c r="K1" s="43"/>
       <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-    </row>
-    <row r="2" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44"/>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -4234,135 +4283,125 @@
       <c r="J2" s="44"/>
       <c r="K2" s="44"/>
       <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-    </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:12" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="378" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="L4" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="B3" s="7" t="s">
+    </row>
+    <row r="5" spans="1:12" ht="369.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>262</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="F5" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="G5" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="378" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" s="32" t="s">
+      <c r="H5" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="I5" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="J5" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="K5" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="G4" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>218</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>213</v>
-      </c>
-      <c r="M4" s="32" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="369.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="31" t="s">
+      <c r="L5" s="31" t="s">
         <v>208</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>217</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>223</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="K5" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="L5" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>222</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4399,7 +4438,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -4448,7 +4487,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>21</v>
@@ -4474,10 +4513,10 @@
         <v>23</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L3" s="97" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4485,10 +4524,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D4" s="32">
         <v>1</v>
@@ -4511,7 +4550,7 @@
         <v>22</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4519,7 +4558,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>21</v>
@@ -4545,7 +4584,7 @@
         <v>23</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="36" x14ac:dyDescent="0.3">
@@ -4553,10 +4592,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D6" s="32">
         <v>1</v>
@@ -4579,7 +4618,7 @@
         <v>23</v>
       </c>
       <c r="J6" s="32" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4587,7 +4626,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>21</v>
@@ -4613,7 +4652,7 @@
         <v>23</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4621,10 +4660,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D8" s="32">
         <v>1</v>
@@ -4647,7 +4686,7 @@
         <v>24</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4655,7 +4694,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>21</v>
@@ -4681,7 +4720,7 @@
         <v>23</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="36" x14ac:dyDescent="0.3">
@@ -4689,10 +4728,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="32">
         <v>1</v>
@@ -4712,10 +4751,10 @@
         <v>10</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4723,7 +4762,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>21</v>
@@ -4749,7 +4788,7 @@
         <v>23</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4757,10 +4796,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D12" s="32">
         <v>1</v>
@@ -4780,10 +4819,10 @@
         <v>25</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4791,7 +4830,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>21</v>
@@ -4817,7 +4856,7 @@
         <v>23</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="90" x14ac:dyDescent="0.3">
@@ -4825,10 +4864,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D14" s="32">
         <v>1</v>
@@ -4851,7 +4890,7 @@
         <v>22</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4859,7 +4898,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>21</v>
@@ -4885,7 +4924,7 @@
         <v>24</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="72" x14ac:dyDescent="0.3">
@@ -4893,10 +4932,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D16" s="32">
         <v>1</v>
@@ -4916,10 +4955,10 @@
         <v>4</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J16" s="32" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.3">
@@ -4927,7 +4966,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>21</v>
@@ -4953,7 +4992,7 @@
         <v>23</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -4961,10 +5000,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D18" s="32">
         <v>1</v>
@@ -4987,7 +5026,7 @@
         <v>24</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -5038,7 +5077,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -5087,44 +5126,44 @@
         <v>1</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>111</v>
+        <v>250</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" s="31">
         <v>1</v>
       </c>
       <c r="E3" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="31">
         <v>5</v>
       </c>
       <c r="G3" s="31">
         <f>E3*F3</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H3" s="31">
         <f>G3</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>106</v>
+        <v>251</v>
       </c>
       <c r="L3" s="97" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="54" x14ac:dyDescent="0.3">
       <c r="A4" s="32">
         <v>2</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>112</v>
+        <v>252</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>21</v>
@@ -5133,58 +5172,58 @@
         <v>1</v>
       </c>
       <c r="E4" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" s="32">
         <f t="shared" ref="G4" si="0">E4*F4</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H4" s="32">
         <f t="shared" ref="H4:H10" si="1">G4</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I4" s="32" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A5" s="31">
         <v>3</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>25</v>
+        <v>254</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D5" s="31">
         <v>1</v>
       </c>
       <c r="E5" s="31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F5" s="31">
         <v>5</v>
       </c>
       <c r="G5" s="31">
         <f>E5*F5</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H5" s="31">
         <f>G5</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>26</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="36" x14ac:dyDescent="0.3">
@@ -5192,7 +5231,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>114</v>
+        <v>269</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>21</v>
@@ -5204,55 +5243,55 @@
         <v>1</v>
       </c>
       <c r="F6" s="32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G6" s="32">
         <f t="shared" ref="G6:G10" si="2">E6*F6</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6" s="32">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I6" s="32" t="s">
         <v>24</v>
       </c>
       <c r="J6" s="32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="31">
         <v>5</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>115</v>
+        <v>256</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D7" s="31">
         <v>1</v>
       </c>
       <c r="E7" s="31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7" s="31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G7" s="31">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H7" s="31">
         <f>G7</f>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>116</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -5260,7 +5299,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>21</v>
@@ -5286,7 +5325,7 @@
         <v>23</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -5294,10 +5333,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>119</v>
+        <v>258</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D9" s="31">
         <v>1</v>
@@ -5306,29 +5345,29 @@
         <v>1</v>
       </c>
       <c r="F9" s="31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G9" s="31">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="31">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I9" s="31" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="90" x14ac:dyDescent="0.3">
       <c r="A10" s="32">
         <v>8</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>121</v>
+        <v>270</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>21</v>
@@ -5340,21 +5379,21 @@
         <v>1</v>
       </c>
       <c r="F10" s="32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G10" s="32">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10" s="32">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I10" s="32" t="s">
         <v>24</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>122</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -5362,41 +5401,41 @@
         <v>9</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>117</v>
+        <v>260</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D11" s="31">
         <v>1</v>
       </c>
       <c r="E11" s="31">
-        <v>0.33333333333333298</v>
+        <v>4</v>
       </c>
       <c r="F11" s="31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G11" s="31">
         <f t="shared" ref="G11:G18" si="3">E11*F11</f>
-        <v>1.666666666666665</v>
+        <v>12</v>
       </c>
       <c r="H11" s="31">
         <f t="shared" ref="H11:H18" si="4">G11</f>
-        <v>1.666666666666665</v>
+        <v>12</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.3">
       <c r="A12" s="32">
         <v>10</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>119</v>
+        <v>272</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>21</v>
@@ -5405,58 +5444,58 @@
         <v>1</v>
       </c>
       <c r="E12" s="32">
-        <v>-0.16666666666666699</v>
+        <v>1</v>
       </c>
       <c r="F12" s="32">
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="G12" s="32">
         <f t="shared" si="3"/>
-        <v>-0.91666666666666841</v>
+        <v>2</v>
       </c>
       <c r="H12" s="32">
         <f t="shared" si="4"/>
-        <v>-0.91666666666666841</v>
+        <v>2</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="54" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="31">
         <v>11</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>121</v>
+        <v>263</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D13" s="31">
         <v>1</v>
       </c>
       <c r="E13" s="31">
-        <v>-0.66666666666666696</v>
+        <v>5</v>
       </c>
       <c r="F13" s="31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" s="31">
         <f t="shared" si="3"/>
-        <v>-4.0000000000000018</v>
+        <v>25</v>
       </c>
       <c r="H13" s="31">
         <f t="shared" si="4"/>
-        <v>-4.0000000000000018</v>
+        <v>25</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>122</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -5464,7 +5503,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>117</v>
+        <v>274</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>21</v>
@@ -5473,58 +5512,58 @@
         <v>1</v>
       </c>
       <c r="E14" s="32">
-        <v>-1.1666666666666701</v>
+        <v>1</v>
       </c>
       <c r="F14" s="32">
-        <v>6.5</v>
+        <v>1</v>
       </c>
       <c r="G14" s="32">
         <f t="shared" si="3"/>
-        <v>-7.5833333333333552</v>
+        <v>1</v>
       </c>
       <c r="H14" s="32">
         <f t="shared" si="4"/>
-        <v>-7.5833333333333552</v>
+        <v>1</v>
       </c>
       <c r="I14" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="36" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="54" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
         <v>13</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>119</v>
+        <v>265</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D15" s="31">
         <v>1</v>
       </c>
       <c r="E15" s="31">
-        <v>-1.6666666666666701</v>
+        <v>5</v>
       </c>
       <c r="F15" s="31">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G15" s="31">
         <f t="shared" si="3"/>
-        <v>-11.666666666666691</v>
+        <v>15</v>
       </c>
       <c r="H15" s="31">
         <f t="shared" si="4"/>
-        <v>-11.666666666666691</v>
+        <v>15</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>120</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -5532,7 +5571,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>121</v>
+        <v>276</v>
       </c>
       <c r="C16" s="32" t="s">
         <v>21</v>
@@ -5541,66 +5580,66 @@
         <v>1</v>
       </c>
       <c r="E16" s="32">
-        <v>-2.1666666666666701</v>
+        <v>1</v>
       </c>
       <c r="F16" s="32">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="G16" s="32">
         <f t="shared" si="3"/>
-        <v>-16.250000000000025</v>
+        <v>5</v>
       </c>
       <c r="H16" s="32">
         <f t="shared" si="4"/>
-        <v>-16.250000000000025</v>
+        <v>5</v>
       </c>
       <c r="I16" s="32" t="s">
         <v>24</v>
       </c>
       <c r="J16" s="32" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>15</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>117</v>
+        <v>267</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D17" s="31">
         <v>1</v>
       </c>
       <c r="E17" s="31">
-        <v>-2.6666666666666701</v>
+        <v>3</v>
       </c>
       <c r="F17" s="31">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G17" s="31">
         <f t="shared" si="3"/>
-        <v>-21.333333333333361</v>
+        <v>9</v>
       </c>
       <c r="H17" s="31">
         <f t="shared" si="4"/>
-        <v>-21.333333333333361</v>
+        <v>9</v>
       </c>
       <c r="I17" s="31" t="s">
         <v>23</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="32">
         <v>16</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>119</v>
+        <v>278</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>21</v>
@@ -5609,24 +5648,24 @@
         <v>1</v>
       </c>
       <c r="E18" s="32">
-        <v>-3.1666666666666701</v>
+        <v>2</v>
       </c>
       <c r="F18" s="32">
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="G18" s="32">
         <f t="shared" si="3"/>
-        <v>-26.916666666666696</v>
+        <v>10</v>
       </c>
       <c r="H18" s="32">
         <f t="shared" si="4"/>
-        <v>-26.916666666666696</v>
+        <v>10</v>
       </c>
       <c r="I18" s="32" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>120</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -5664,45 +5703,45 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B6" s="16"/>
     </row>
@@ -5712,45 +5751,45 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="19"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>12</v>
@@ -5762,45 +5801,45 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="19"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>12</v>
@@ -5812,45 +5851,45 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="19"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>12</v>
@@ -5862,45 +5901,45 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" s="19"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>12</v>
@@ -5912,57 +5951,57 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" s="19"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B41" s="15"/>
     </row>
     <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="11"/>
       <c r="B42" s="76" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B43" s="21" t="s">
         <v>13</v>
@@ -5996,38 +6035,38 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6036,45 +6075,45 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="19"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>12</v>
@@ -6086,45 +6125,45 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B14" s="19"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>13</v>
@@ -6136,45 +6175,45 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B21" s="19"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>12</v>
@@ -6186,45 +6225,45 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B28" s="19"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>12</v>
@@ -6236,45 +6275,45 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B35" s="19"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>13</v>
@@ -6286,45 +6325,45 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B42" s="19"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>12</v>
@@ -6332,30 +6371,30 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6364,45 +6403,45 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B53" s="14"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>12</v>
@@ -6414,45 +6453,45 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B60" s="19"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B65" s="17" t="s">
         <v>12</v>
@@ -6464,45 +6503,45 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B67" s="19"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B72" s="17" t="s">
         <v>12</v>
@@ -6514,45 +6553,45 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B74" s="19"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>12</v>
@@ -6564,45 +6603,45 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B81" s="19"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B82" s="20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B83" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B84" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B85" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>12</v>
@@ -6614,45 +6653,45 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="18" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B88" s="19"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B89" s="20" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B90" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B91" s="20" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B92" s="20" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B93" s="21" t="s">
         <v>13</v>
@@ -6672,7 +6711,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:I1"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -6691,7 +6730,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -6704,212 +6743,212 @@
     </row>
     <row r="2" spans="1:9" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="78" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C2" s="79"/>
       <c r="D2" s="78" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="F2" s="79"/>
       <c r="G2" s="78" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.3">
       <c r="A3" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>138</v>
+        <v>125</v>
+      </c>
+      <c r="B3" s="98" t="s">
+        <v>142</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D3" s="80" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="F3" s="81" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="G3" s="80" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="I3" s="81" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="82" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C4" s="83" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="F4" s="83" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="G4" s="82" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="I4" s="83" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="80" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C5" s="84"/>
       <c r="D5" s="80" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="F5" s="84"/>
       <c r="G5" s="80" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H5" s="51" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="I5" s="84"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="82" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="85"/>
       <c r="D6" s="82" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="85"/>
       <c r="G6" s="82" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="85"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="80" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B7" s="53"/>
       <c r="C7" s="86"/>
       <c r="D7" s="80" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E7" s="53"/>
       <c r="F7" s="86"/>
       <c r="G7" s="80" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="86"/>
     </row>
     <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="82" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C8" s="87"/>
       <c r="D8" s="82" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="F8" s="87"/>
       <c r="G8" s="82" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="H8" s="54" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="I8" s="87"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="88" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="89"/>
       <c r="D9" s="88" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="E9" s="55"/>
       <c r="F9" s="89"/>
       <c r="G9" s="88" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H9" s="55"/>
       <c r="I9" s="89"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="90" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B10" s="56"/>
       <c r="C10" s="91"/>
       <c r="D10" s="90" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E10" s="56"/>
       <c r="F10" s="91"/>
       <c r="G10" s="90" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="H10" s="56"/>
       <c r="I10" s="91"/>
     </row>
     <row r="11" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="92" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B11" s="49"/>
       <c r="C11" s="93"/>
       <c r="D11" s="92" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E11" s="49"/>
       <c r="F11" s="93"/>
       <c r="G11" s="92" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="H11" s="49"/>
       <c r="I11" s="93"/>
@@ -6917,7 +6956,7 @@
     <row r="13" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="94" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="E14" s="94"/>
       <c r="F14" s="94"/>
@@ -6965,7 +7004,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:I1"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -6984,7 +7023,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -6997,212 +7036,212 @@
     </row>
     <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="78" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C2" s="79"/>
       <c r="D2" s="78" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F2" s="79"/>
       <c r="G2" s="78" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.3">
       <c r="A3" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>138</v>
+        <v>125</v>
+      </c>
+      <c r="B3" s="98" t="s">
+        <v>142</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D3" s="80" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="F3" s="81" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="G3" s="80" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="I3" s="81" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A4" s="82" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C4" s="83" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F4" s="83" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="G4" s="82" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="I4" s="83" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="80" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C5" s="84"/>
       <c r="D5" s="80" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F5" s="84"/>
       <c r="G5" s="80" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H5" s="51" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="I5" s="84"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="82" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="85"/>
       <c r="D6" s="82" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="85"/>
       <c r="G6" s="82" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="85"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="80" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B7" s="53"/>
       <c r="C7" s="86"/>
       <c r="D7" s="80" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E7" s="53"/>
       <c r="F7" s="86"/>
       <c r="G7" s="80" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="86"/>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.3">
       <c r="A8" s="82" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C8" s="87"/>
       <c r="D8" s="82" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="F8" s="87"/>
       <c r="G8" s="82" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H8" s="54" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="I8" s="87"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="88" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="89"/>
       <c r="D9" s="88" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="E9" s="55"/>
       <c r="F9" s="89"/>
       <c r="G9" s="88" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="H9" s="55"/>
       <c r="I9" s="89"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="90" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B10" s="56"/>
       <c r="C10" s="91"/>
       <c r="D10" s="90" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E10" s="56"/>
       <c r="F10" s="91"/>
       <c r="G10" s="90" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="H10" s="56"/>
       <c r="I10" s="91"/>
     </row>
     <row r="11" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="92" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B11" s="49"/>
       <c r="C11" s="93"/>
       <c r="D11" s="92" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E11" s="49"/>
       <c r="F11" s="93"/>
       <c r="G11" s="92" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="H11" s="49"/>
       <c r="I11" s="93"/>
@@ -7210,7 +7249,7 @@
     <row r="13" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="94" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E14" s="94"/>
       <c r="F14" s="94"/>
@@ -7228,84 +7267,84 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B24" s="66" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C24" s="67"/>
     </row>
     <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B27" s="68" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C27" s="69"/>
     </row>
     <row r="28" spans="1:3" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B28" s="70"/>
       <c r="C28" s="71"/>
     </row>
     <row r="29" spans="1:3" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B29" s="60"/>
       <c r="C29" s="62"/>
     </row>
     <row r="30" spans="1:3" ht="108" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B30" s="72" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C30" s="59"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="73" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B31" s="74"/>
       <c r="C31" s="75"/>
     </row>
     <row r="32" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="57" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B32" s="58"/>
       <c r="C32" s="59"/>
     </row>
     <row r="33" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="60" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B33" s="61"/>
       <c r="C33" s="62"/>
@@ -7362,7 +7401,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="40" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -7370,37 +7409,37 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="37" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="38" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -7408,7 +7447,7 @@
     </row>
     <row r="11" spans="1:1" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="41" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✏️  Fixing typos in progress report and Excel file
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA238C6-B749-4D79-8968-1FC723B3AE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B5B1CC-A3D4-4174-A026-4B1DA3DBD978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="893" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
@@ -2589,29 +2589,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Título:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> No se convierte una cantidad elevada de dólares a pesos colombianos</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Resumen:</t>
     </r>
     <r>
@@ -2739,29 +2716,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Título:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Se muestra un error al usar la coma como separador decimal</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Resumen:</t>
     </r>
     <r>
@@ -2866,29 +2820,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Título:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> No se muestra la tasa de cambio para la fecha antigua especificada</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Resumen:</t>
     </r>
     <r>
@@ -3087,6 +3018,84 @@
   </si>
   <si>
     <t>Verificar que el campo To es sensible a mayúsculas</t>
+  </si>
+  <si>
+    <r>
+      <t>Título:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> No se convierte una cantidad elevada de dólares a pesos colombianos</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Título:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Se muestra un error al usar la coma como separador decimal</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Título:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> No se muestra la tasa de cambio para la fecha antigua especificada</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3741,7 +3750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3807,6 +3816,45 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3825,63 +3873,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3891,45 +3882,56 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4788,32 +4790,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
     </row>
     <row r="2" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -4968,18 +4970,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -5046,7 +5048,7 @@
       <c r="J3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="31" t="s">
         <v>103</v>
       </c>
     </row>
@@ -5607,18 +5609,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -5685,7 +5687,7 @@
       <c r="J3" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="31" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6235,13 +6237,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="33" t="s">
         <v>155</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="33" t="s">
         <v>155</v>
       </c>
       <c r="D1" s="19" t="s">
@@ -6409,10 +6411,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -6495,10 +6497,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
@@ -6509,7 +6511,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -6537,7 +6539,7 @@
         <v>28</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -6551,7 +6553,7 @@
         <v>29</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -6561,7 +6563,6 @@
       <c r="B26" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="C26" s="66"/>
       <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6574,28 +6575,28 @@
       <c r="C27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="68" t="s">
+      <c r="D27" s="39" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
+      <c r="A28" s="44"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="45"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -6617,13 +6618,13 @@
         <v>28</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -6631,47 +6632,47 @@
         <v>29</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="39" t="s">
         <v>272</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="39" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="31"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="45"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -6685,7 +6686,7 @@
         <v>32</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -6693,13 +6694,13 @@
         <v>28</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -6707,47 +6708,47 @@
         <v>29</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="68" t="s">
+      <c r="B39" s="39" t="s">
         <v>272</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="68" t="s">
+      <c r="D39" s="39" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="32"/>
+      <c r="A40" s="44"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="45"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -6755,7 +6756,7 @@
         <v>32</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>32</v>
@@ -6769,13 +6770,13 @@
         <v>28</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -6783,47 +6784,47 @@
         <v>29</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B45" s="68" t="s">
+      <c r="B45" s="39" t="s">
         <v>272</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="68" t="s">
+      <c r="D45" s="39" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="31"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="32"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="45"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -6845,13 +6846,13 @@
         <v>28</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -6859,47 +6860,47 @@
         <v>29</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B51" s="68" t="s">
+      <c r="B51" s="39" t="s">
         <v>272</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="68" t="s">
+      <c r="D51" s="39" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="31"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="32"/>
+      <c r="A52" s="44"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="45"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -6921,13 +6922,13 @@
         <v>28</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -6935,47 +6936,47 @@
         <v>29</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="68" t="s">
+      <c r="B57" s="39" t="s">
         <v>272</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="68" t="s">
+      <c r="D57" s="39" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="31"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="32"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="45"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -6997,13 +6998,13 @@
         <v>28</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -7011,47 +7012,47 @@
         <v>29</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B63" s="68" t="s">
+      <c r="B63" s="39" t="s">
         <v>272</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D63" s="68" t="s">
+      <c r="D63" s="39" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="31"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="32"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="45"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="45"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -7073,13 +7074,13 @@
         <v>28</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -7087,39 +7088,39 @@
         <v>29</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="68" t="s">
+      <c r="B69" s="39" t="s">
         <v>272</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D69" s="68" t="s">
+      <c r="D69" s="39" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="31"/>
-      <c r="B70" s="32"/>
+      <c r="A70" s="44"/>
+      <c r="B70" s="45"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -7135,7 +7136,7 @@
         <v>28</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -7143,19 +7144,25 @@
         <v>29</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B75" s="68" t="s">
+      <c r="B75" s="39" t="s">
         <v>272</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A64:B64"/>
@@ -7169,12 +7176,6 @@
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7199,13 +7200,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="33" t="s">
         <v>155</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="33" t="s">
         <v>155</v>
       </c>
       <c r="D1" s="19" t="s">
@@ -7397,10 +7398,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -7489,7 +7490,6 @@
       <c r="B23" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C23" s="66"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -7504,11 +7504,11 @@
     </row>
     <row r="25" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="27" t="s">
         <v>220</v>
       </c>
       <c r="C25" s="6"/>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="27" t="s">
         <v>221</v>
       </c>
     </row>
@@ -7527,10 +7527,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
@@ -7613,13 +7613,13 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="33" t="s">
         <v>155</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="33" t="s">
         <v>155</v>
       </c>
       <c r="D34" s="19" t="s">
@@ -7793,7 +7793,6 @@
       <c r="B47" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C47" s="66"/>
       <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7811,10 +7810,10 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="31"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="32"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="45"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
@@ -7884,7 +7883,6 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
-      <c r="B55" s="66"/>
       <c r="C55" s="6" t="s">
         <v>29</v>
       </c>
@@ -7904,11 +7902,11 @@
     </row>
     <row r="57" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="27" t="s">
         <v>232</v>
       </c>
       <c r="C57" s="6"/>
-      <c r="D57" s="35" t="s">
+      <c r="D57" s="27" t="s">
         <v>222</v>
       </c>
     </row>
@@ -7927,10 +7925,10 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="31"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="32"/>
+      <c r="A59" s="44"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="45"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
@@ -7991,16 +7989,15 @@
       <c r="B64" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="C64" s="58" t="s">
+      <c r="C64" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D64" s="59" t="s">
+      <c r="D64" s="8" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="13"/>
-      <c r="B65" s="66"/>
       <c r="C65" s="6" t="s">
         <v>29</v>
       </c>
@@ -8020,7 +8017,7 @@
       <c r="A67" s="6"/>
       <c r="B67" s="8"/>
       <c r="C67" s="6"/>
-      <c r="D67" s="35" t="s">
+      <c r="D67" s="27" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8081,203 +8078,203 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="55"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="F2" s="58"/>
+      <c r="G2" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>349</v>
+      </c>
+      <c r="I2" s="58"/>
+    </row>
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="62" t="s">
-        <v>305</v>
-      </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="62" t="s">
-        <v>310</v>
-      </c>
-      <c r="I2" s="51"/>
-    </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.3">
-      <c r="A3" s="61" t="s">
-        <v>234</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="63" t="s">
-        <v>300</v>
-      </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="36" t="s">
         <v>234</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="63" t="s">
-        <v>306</v>
-      </c>
-      <c r="G3" s="61" t="s">
+      <c r="F3" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="G3" s="36" t="s">
         <v>234</v>
       </c>
       <c r="H3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="63" t="s">
-        <v>311</v>
+      <c r="I3" s="37" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="29" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="29" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="29" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="65" t="s">
-        <v>304</v>
-      </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="61" t="s">
+      <c r="B5" s="53" t="s">
+        <v>303</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="53" t="s">
+        <v>307</v>
+      </c>
+      <c r="F5" s="54"/>
+      <c r="G5" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="53" t="s">
         <v>309</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="65" t="s">
-        <v>312</v>
-      </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="B6" s="55"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="38" t="s">
+        <v>300</v>
+      </c>
+      <c r="H6" s="55"/>
+      <c r="I6" s="56"/>
+    </row>
+    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="67" t="s">
-        <v>301</v>
-      </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="40"/>
-    </row>
-    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="61" t="s">
+      <c r="B7" s="59" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="64" t="s">
-        <v>303</v>
-      </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="61" t="s">
-        <v>307</v>
-      </c>
-      <c r="E7" s="64" t="s">
-        <v>308</v>
-      </c>
-      <c r="F7" s="57"/>
-      <c r="G7" s="61" t="s">
-        <v>313</v>
-      </c>
-      <c r="H7" s="64" t="s">
-        <v>314</v>
-      </c>
-      <c r="I7" s="57"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>306</v>
+      </c>
+      <c r="F7" s="60"/>
+      <c r="G7" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>311</v>
+      </c>
+      <c r="I7" s="60"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="41" t="s">
+      <c r="B8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="41" t="s">
+      <c r="E8" s="62"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="42"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
     </row>
     <row r="9" spans="1:9" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="52" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="46" t="s">
         <v>297</v>
       </c>
-      <c r="E9" s="53"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="52" t="s">
+      <c r="E9" s="47"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="46" t="s">
         <v>298</v>
       </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="54"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="48"/>
     </row>
     <row r="11" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
     </row>
     <row r="14" spans="1:9" ht="55.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:9" ht="88.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8287,6 +8284,7 @@
     <row r="20" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="A1:I1"/>
@@ -8303,7 +8301,6 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8337,203 +8334,203 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="55"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="57" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="60" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="64" t="s">
         <v>246</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="60" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="35" t="s">
         <v>233</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="64" t="s">
         <v>256</v>
       </c>
-      <c r="I2" s="51"/>
+      <c r="I2" s="58"/>
     </row>
     <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.3">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="36" t="s">
         <v>234</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="F3" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="G3" s="61" t="s">
+      <c r="G3" s="36" t="s">
         <v>234</v>
       </c>
       <c r="H3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="63" t="s">
+      <c r="I3" s="37" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="29" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="29" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="29" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="53" t="s">
         <v>268</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="61" t="s">
+      <c r="C5" s="54"/>
+      <c r="D5" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="53" t="s">
         <v>249</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="36" t="s">
+      <c r="F5" s="54"/>
+      <c r="G5" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="65" t="s">
+      <c r="H5" s="53" t="s">
         <v>258</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="67" t="s">
+      <c r="B6" s="55"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="37" t="s">
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="40"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="56"/>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.3">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="36" t="s">
         <v>238</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="59" t="s">
         <v>269</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="61" t="s">
+      <c r="C7" s="60"/>
+      <c r="D7" s="36" t="s">
         <v>250</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="F7" s="57"/>
-      <c r="G7" s="61" t="s">
+      <c r="F7" s="60"/>
+      <c r="G7" s="36" t="s">
         <v>259</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="65" t="s">
         <v>260</v>
       </c>
-      <c r="I7" s="57"/>
+      <c r="I7" s="60"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="41" t="s">
+      <c r="B8" s="62"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="61" t="s">
         <v>252</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="41" t="s">
+      <c r="E8" s="62"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="61" t="s">
         <v>255</v>
       </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="42"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
     </row>
     <row r="9" spans="1:9" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="52" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="46" t="s">
         <v>253</v>
       </c>
-      <c r="E9" s="53"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="52" t="s">
+      <c r="E9" s="47"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="46" t="s">
         <v>254</v>
       </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="54"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="48"/>
     </row>
     <row r="11" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
     </row>
     <row r="14" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8598,6 +8595,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A8:C8"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B5:C6"/>
@@ -8614,7 +8612,6 @@
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>